<commit_message>
Update dial specifications and workflows: Modify dial.ipynb to reflect new input and output paths for MI dials, adjust execution counts, and update command structures in quant_workflows_notebook.ipynb for consistency. Revise JSON specifications for MI and non-QM dials, including version updates and additional model details. Enhance stacr specifications with new model details and correct dial values for improved accuracy.
</commit_message>
<xml_diff>
--- a/dial/outputs/dial_ratio_by_deal_6M_edit - Copy.xlsx
+++ b/dial/outputs/dial_ratio_by_deal_6M_edit - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hzeng\Desktop\howard-toolbox\dial\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE4362D-9772-4649-83BA-0F8C421DE32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F64B69-88D9-49D1-91AA-AE23828F493B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10275" yWindow="-21750" windowWidth="49725" windowHeight="21285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15345" yWindow="-150" windowWidth="44655" windowHeight="21285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STACR" sheetId="1" r:id="rId1"/>
@@ -794,9 +794,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,11 +1682,11 @@
         <v>1.6427863217142289</v>
       </c>
       <c r="H30" s="22">
-        <v>6.1214364610666001</v>
+        <v>1.75</v>
       </c>
       <c r="I30" s="4">
         <f t="shared" si="0"/>
-        <v>4.4786501393523714</v>
+        <v>0.10721367828577111</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1877,9 +1877,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2525,11 +2525,11 @@
         <v>1.6240864380587079</v>
       </c>
       <c r="H22" s="22">
-        <v>4.1537762141474852</v>
+        <v>1.75</v>
       </c>
       <c r="I22" s="4">
         <f t="shared" si="0"/>
-        <v>2.5296897760887775</v>
+        <v>0.12591356194129211</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2705,11 +2705,11 @@
         <v>1.6370254731010681</v>
       </c>
       <c r="H28" s="22">
-        <v>4.6777567883175477</v>
+        <v>1.75</v>
       </c>
       <c r="I28" s="4">
         <f t="shared" si="0"/>
-        <v>3.0407313152164797</v>
+        <v>0.11297452689893195</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2895,7 +2895,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:I42"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3755,11 +3755,11 @@
         <v>1.0087302754317311</v>
       </c>
       <c r="H29" s="8">
-        <v>1.0906443829268246</v>
+        <v>1.09064438292682</v>
       </c>
       <c r="I29" s="4">
         <f t="shared" si="0"/>
-        <v>8.1914107495093536E-2</v>
+        <v>8.1914107495088873E-2</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3785,11 +3785,11 @@
         <v>1</v>
       </c>
       <c r="H30" s="5">
-        <v>1.1651372000584392</v>
+        <v>1.1651372000584399</v>
       </c>
       <c r="I30" s="4">
         <f t="shared" si="0"/>
-        <v>-0.42964892796191667</v>
+        <v>-0.42964892796191601</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3815,11 +3815,11 @@
         <v>1.3152958851067931</v>
       </c>
       <c r="H31" s="8">
-        <v>1.3456222354051692</v>
+        <v>1.3456222354051699</v>
       </c>
       <c r="I31" s="4">
         <f t="shared" si="0"/>
-        <v>3.0326350298376159E-2</v>
+        <v>3.0326350298376825E-2</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3845,11 +3845,11 @@
         <v>1.540662781470777</v>
       </c>
       <c r="H32" s="5">
-        <v>1.6062523236577366</v>
+        <v>1.60625232365774</v>
       </c>
       <c r="I32" s="4">
         <f t="shared" si="0"/>
-        <v>6.5589542186959671E-2</v>
+        <v>6.5589542186963001E-2</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3875,11 +3875,11 @@
         <v>0.74075833503750932</v>
       </c>
       <c r="H33" s="8">
-        <v>0.73706281062687973</v>
+        <v>0.73706281062687995</v>
       </c>
       <c r="I33" s="4">
         <f t="shared" si="0"/>
-        <v>-3.6955244106295915E-3</v>
+        <v>-3.6955244106293694E-3</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3965,11 +3965,11 @@
         <v>0.35590806731908381</v>
       </c>
       <c r="H36" s="22">
-        <v>8.5714379190687737E-3</v>
+        <v>0.25</v>
       </c>
       <c r="I36" s="4">
         <f t="shared" si="0"/>
-        <v>-0.34733662940001503</v>
+        <v>-0.10590806731908381</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3995,11 +3995,11 @@
         <v>0.44462048265946652</v>
       </c>
       <c r="H37" s="8">
-        <v>0.24619312344272939</v>
+        <v>0.25</v>
       </c>
       <c r="I37" s="4">
         <f t="shared" si="0"/>
-        <v>-0.19842735921673713</v>
+        <v>-0.19462048265946652</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4025,11 +4025,11 @@
         <v>0.98777793290015015</v>
       </c>
       <c r="H38" s="5">
-        <v>0.48833040506159509</v>
+        <v>0.48833040506159497</v>
       </c>
       <c r="I38" s="4">
         <f t="shared" si="0"/>
-        <v>-0.49944752783855506</v>
+        <v>-0.49944752783855517</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -4115,11 +4115,11 @@
         <v>1</v>
       </c>
       <c r="H41" s="8">
-        <v>1.0957770660791653</v>
+        <v>1.0957770660791699</v>
       </c>
       <c r="I41" s="4">
         <f t="shared" si="0"/>
-        <v>9.4862258961145196E-2</v>
+        <v>9.4862258961149859E-2</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -4145,11 +4145,11 @@
         <v>0.35328227106859889</v>
       </c>
       <c r="H42" s="22">
-        <v>5.4697882175982968E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I42" s="4">
         <f t="shared" si="0"/>
-        <v>-0.2985843888926159</v>
+        <v>-0.10328227106859889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update dial specifications and workflows: Adjust execution counts in dial.ipynb for consistency, modify paths for MI dials, and revise command structures in quant_workflows_notebook.ipynb. Update JSON specifications for MI and non-QM dials, including new model details and corrected dial values for improved accuracy. Remove outdated image assets from the emailer module to streamline functionality.
</commit_message>
<xml_diff>
--- a/dial/outputs/dial_ratio_by_deal_6M_edit - Copy.xlsx
+++ b/dial/outputs/dial_ratio_by_deal_6M_edit - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hzeng\Desktop\howard-toolbox\dial\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F64B69-88D9-49D1-91AA-AE23828F493B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBAC1AD-303F-45B1-9E0E-EB2ED417995A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15345" yWindow="-150" windowWidth="44655" windowHeight="21285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10275" yWindow="-21750" windowWidth="49725" windowHeight="21285" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STACR" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="NONQM" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CAS!$A$2:$I$32</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NONQM!$A$2:$I$42</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">STACR!$A$2:$I$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CAS!$A$2:$G$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NONQM!$A$2:$G$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">STACR!$A$2:$G$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="66">
   <si>
     <t>STACR</t>
   </si>
@@ -58,12 +58,6 @@
   </si>
   <si>
     <t>Current_Dial</t>
-  </si>
-  <si>
-    <t>Implied_Dial</t>
-  </si>
-  <si>
-    <t>Proposed_Dial</t>
   </si>
   <si>
     <t>Dial Diff (New - Current)</t>
@@ -253,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,24 +272,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -410,9 +386,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -447,41 +423,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -792,11 +746,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,31 +759,27 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -840,25 +790,19 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>6</v>
+      <c r="F2" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3">
@@ -867,26 +811,20 @@
       <c r="E3" s="5">
         <v>0.86212922230984146</v>
       </c>
-      <c r="F3" s="13">
-        <v>1.2288966793154441</v>
-      </c>
-      <c r="G3" s="11">
+      <c r="F3" s="11">
         <v>0.95899999999999996</v>
       </c>
-      <c r="H3" s="11">
-        <v>0.95899999999999996</v>
-      </c>
-      <c r="I3" s="4">
-        <f>H3-E3</f>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G35" si="0">F3-E3</f>
         <v>9.6870777690158505E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3">
@@ -895,29 +833,23 @@
       <c r="E4" s="5">
         <v>0.86212922230984146</v>
       </c>
-      <c r="F4" s="17">
-        <v>1.2288966793154441</v>
-      </c>
-      <c r="G4" s="11">
+      <c r="F4" s="11">
         <v>1.75</v>
       </c>
-      <c r="H4" s="11">
-        <v>1.75</v>
-      </c>
-      <c r="I4" s="4">
-        <f t="shared" ref="I4:I35" si="0">H4-E4</f>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
         <v>0.88787077769015854</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" s="7">
         <v>250000</v>
@@ -925,29 +857,23 @@
       <c r="E5" s="8">
         <v>1.194505303873032</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="11">
         <v>1.2090000000000001</v>
       </c>
-      <c r="G5" s="11">
-        <v>1.2090000000000001</v>
-      </c>
-      <c r="H5" s="11">
-        <v>1.2090000000000001</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="G5" s="4">
         <f t="shared" si="0"/>
         <v>1.4494696126968076E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" s="7">
         <v>250000</v>
@@ -955,29 +881,23 @@
       <c r="E6" s="8">
         <v>1.194505303873032</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="11">
         <v>0.76900000000000002</v>
       </c>
-      <c r="G6" s="11">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="H6" s="11">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="I6" s="4">
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>-0.42550530387303198</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D7" s="3">
         <v>65363</v>
@@ -985,29 +905,23 @@
       <c r="E7" s="5">
         <v>0.78783123830167434</v>
       </c>
-      <c r="F7" s="17">
-        <v>0.81058378867657599</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.78783123830167434</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.78783123830167434</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="5">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>2.3168761698325713E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="D8" s="7">
         <v>65363</v>
@@ -1015,29 +929,23 @@
       <c r="E8" s="8">
         <v>1.453172361404018</v>
       </c>
-      <c r="F8" s="18">
-        <v>1.3151039891753009</v>
-      </c>
-      <c r="G8" s="8">
+      <c r="F8" s="8">
         <v>1.3151039891753</v>
       </c>
-      <c r="H8" s="8">
-        <v>1.3151039891753</v>
-      </c>
-      <c r="I8" s="4">
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>-0.13806837222871793</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3">
         <v>65363</v>
@@ -1045,29 +953,23 @@
       <c r="E9" s="5">
         <v>0.58913122925242201</v>
       </c>
-      <c r="F9" s="17">
-        <v>0.68948767601745409</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0.68948767601745398</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.68948767601745398</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="0"/>
-        <v>0.10035644676503197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F9" s="5">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>9.986877074757794E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" s="7">
         <v>18213</v>
@@ -1075,29 +977,23 @@
       <c r="E10" s="8">
         <v>0.90961034143516595</v>
       </c>
-      <c r="F10" s="15">
-        <v>0.85454022157930476</v>
-      </c>
-      <c r="G10" s="8">
-        <v>0.85454022157930498</v>
-      </c>
-      <c r="H10" s="8">
-        <v>0.85454022157930498</v>
-      </c>
-      <c r="I10" s="4">
-        <f t="shared" si="0"/>
-        <v>-5.5070119855860966E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F10" s="8">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.4610341435165966E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D11" s="3">
         <v>18213</v>
@@ -1105,29 +1001,23 @@
       <c r="E11" s="5">
         <v>1.0003164373471489</v>
       </c>
-      <c r="F11" s="13">
-        <v>0.99636191024726295</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1.0003164373471489</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1.0003164373471489</v>
-      </c>
-      <c r="I11" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="5">
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>3.0683562652850993E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" s="7">
         <v>18213</v>
@@ -1135,29 +1025,23 @@
       <c r="E12" s="8">
         <v>0.99965022176862761</v>
       </c>
-      <c r="F12" s="15">
-        <v>1.0306407891709231</v>
-      </c>
-      <c r="G12" s="8">
-        <v>0.99965022176862761</v>
-      </c>
-      <c r="H12" s="8">
-        <v>0.99965022176862761</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F12" s="8">
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>3.1349778231372305E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" s="3">
         <v>18213</v>
@@ -1165,29 +1049,23 @@
       <c r="E13" s="5">
         <v>1.241082438186017</v>
       </c>
-      <c r="F13" s="13">
-        <v>1.228517549372675</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1.241082438186017</v>
-      </c>
-      <c r="H13" s="5">
-        <v>1.241082438186017</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="5">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.2082438186016953E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14" s="7">
         <v>18213</v>
@@ -1195,29 +1073,23 @@
       <c r="E14" s="8">
         <v>0.62024862149950322</v>
       </c>
-      <c r="F14" s="15">
-        <v>0.44183307923031739</v>
-      </c>
-      <c r="G14" s="8">
-        <v>0.44183307923031701</v>
-      </c>
-      <c r="H14" s="8">
-        <v>0.44183307923031701</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" si="0"/>
-        <v>-0.17841554226918621</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F14" s="8">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.2272486214995032</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D15" s="3">
         <v>22578</v>
@@ -1225,29 +1097,23 @@
       <c r="E15" s="5">
         <v>1.1027115790122339</v>
       </c>
-      <c r="F15" s="13">
-        <v>1.0224798890822071</v>
-      </c>
-      <c r="G15" s="5">
-        <v>1.02247988908221</v>
-      </c>
-      <c r="H15" s="5">
-        <v>1.02247988908221</v>
-      </c>
-      <c r="I15" s="4">
-        <f t="shared" si="0"/>
-        <v>-8.0231689930023942E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F15" s="5">
+        <v>1.022</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="0"/>
+        <v>-8.0711579012233914E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="D16" s="7">
         <v>22578</v>
@@ -1255,29 +1121,23 @@
       <c r="E16" s="8">
         <v>1.1064932541760799</v>
       </c>
-      <c r="F16" s="15">
-        <v>1.0992380071723711</v>
-      </c>
-      <c r="G16" s="8">
-        <v>1.1064932541760799</v>
-      </c>
-      <c r="H16" s="8">
-        <v>1.1064932541760799</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F16" s="8">
+        <v>1.099</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.4932541760799332E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D17" s="3">
         <v>22578</v>
@@ -1285,29 +1145,23 @@
       <c r="E17" s="5">
         <v>0.96671086196458822</v>
       </c>
-      <c r="F17" s="13">
-        <v>0.96962986838793197</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0.96671086196458822</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0.96671086196458822</v>
-      </c>
-      <c r="I17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F17" s="5">
+        <v>0.97</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2891380354117539E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D18" s="7">
         <v>22578</v>
@@ -1315,29 +1169,23 @@
       <c r="E18" s="8">
         <v>0.99739489748299182</v>
       </c>
-      <c r="F18" s="15">
-        <v>0.91520352396647675</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0.91520352396647697</v>
-      </c>
-      <c r="H18" s="8">
-        <v>0.91520352396647697</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" si="0"/>
-        <v>-8.2191373516514843E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="8">
+        <v>0.86543611129386899</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.13195878618912282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" s="3">
         <v>22578</v>
@@ -1345,29 +1193,23 @@
       <c r="E19" s="5">
         <v>0.92299111273003953</v>
       </c>
-      <c r="F19" s="13">
-        <v>0.92940693938367958</v>
-      </c>
-      <c r="G19" s="5">
-        <v>0.92299111273003953</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0.92299111273003953</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="5">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="0"/>
+        <v>6.0088872699605167E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D20" s="7">
         <v>22578</v>
@@ -1375,29 +1217,23 @@
       <c r="E20" s="8">
         <v>0.92307089104182338</v>
       </c>
-      <c r="F20" s="15">
-        <v>0.90451716117569358</v>
-      </c>
-      <c r="G20" s="8">
-        <v>0.92307089104182338</v>
-      </c>
-      <c r="H20" s="8">
-        <v>0.92307089104182338</v>
-      </c>
-      <c r="I20" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="8">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="0"/>
+        <v>5.9291089581766654E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D21" s="3">
         <v>22578</v>
@@ -1405,29 +1241,23 @@
       <c r="E21" s="5">
         <v>1.3516255954818159</v>
       </c>
-      <c r="F21" s="13">
-        <v>1.7077763791853791</v>
-      </c>
-      <c r="G21" s="5">
+      <c r="F21" s="5">
         <v>1.7077763791853799</v>
       </c>
-      <c r="H21" s="5">
-        <v>1.7077763791853799</v>
-      </c>
-      <c r="I21" s="4">
+      <c r="G21" s="4">
         <f t="shared" si="0"/>
         <v>0.35615078370356401</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D22" s="7">
         <v>22578</v>
@@ -1435,29 +1265,23 @@
       <c r="E22" s="8">
         <v>1.243178685922967</v>
       </c>
-      <c r="F22" s="15">
-        <v>1.352718341503433</v>
-      </c>
-      <c r="G22" s="8">
+      <c r="F22" s="8">
         <v>1.3527183415034301</v>
       </c>
-      <c r="H22" s="8">
-        <v>1.3527183415034301</v>
-      </c>
-      <c r="I22" s="4">
+      <c r="G22" s="4">
         <f t="shared" si="0"/>
         <v>0.10953965558046308</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D23" s="3">
         <v>22578</v>
@@ -1465,29 +1289,23 @@
       <c r="E23" s="5">
         <v>1.6229757349056171</v>
       </c>
-      <c r="F23" s="13">
-        <v>0.96442946636154736</v>
-      </c>
-      <c r="G23" s="5">
-        <v>1</v>
-      </c>
-      <c r="H23" s="5">
-        <v>1</v>
-      </c>
-      <c r="I23" s="4">
-        <f t="shared" si="0"/>
-        <v>-0.62297573490561708</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="5">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.65897573490561712</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D24" s="7">
         <v>4512</v>
@@ -1495,29 +1313,23 @@
       <c r="E24" s="8">
         <v>0.96700690225098695</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="13">
         <v>1.037946497645944</v>
       </c>
-      <c r="G24" s="8">
-        <v>1.037946497645944</v>
-      </c>
-      <c r="H24" s="15">
-        <v>1.037946497645944</v>
-      </c>
-      <c r="I24" s="4">
+      <c r="G24" s="4">
         <f t="shared" si="0"/>
         <v>7.0939595394957089E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D25" s="3">
         <v>4512</v>
@@ -1525,29 +1337,23 @@
       <c r="E25" s="5">
         <v>0.81988868832238204</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="12">
         <v>0.66143958184359597</v>
       </c>
-      <c r="G25" s="5">
-        <v>0.66143958184359597</v>
-      </c>
-      <c r="H25" s="13">
-        <v>0.66143958184359597</v>
-      </c>
-      <c r="I25" s="4">
+      <c r="G25" s="4">
         <f t="shared" si="0"/>
         <v>-0.15844910647878607</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D26" s="7">
         <v>4512</v>
@@ -1555,29 +1361,23 @@
       <c r="E26" s="8">
         <v>0.8346374853627172</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="13">
         <v>0.90614298608598054</v>
       </c>
-      <c r="G26" s="8">
-        <v>0.90614298608598054</v>
-      </c>
-      <c r="H26" s="15">
-        <v>0.90614298608598054</v>
-      </c>
-      <c r="I26" s="4">
+      <c r="G26" s="4">
         <f t="shared" si="0"/>
         <v>7.1505500723263338E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D27" s="3">
         <v>4512</v>
@@ -1585,29 +1385,23 @@
       <c r="E27" s="5">
         <v>0.98843923233498565</v>
       </c>
-      <c r="F27" s="13">
-        <v>0.95556210620775972</v>
-      </c>
-      <c r="G27" s="5">
-        <v>0.98843923233498565</v>
-      </c>
-      <c r="H27" s="13">
-        <v>0.95556210620775972</v>
-      </c>
-      <c r="I27" s="4">
-        <f t="shared" si="0"/>
-        <v>-3.2877126127225931E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F27" s="12">
+        <v>0.93827158832211799</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.0167644012867663E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D28" s="7">
         <v>4512</v>
@@ -1615,29 +1409,23 @@
       <c r="E28" s="8">
         <v>1.350988666075484</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="13">
         <v>1.487047447193091</v>
       </c>
-      <c r="G28" s="8">
-        <v>1.4870474471930899</v>
-      </c>
-      <c r="H28" s="15">
-        <v>1.487047447193091</v>
-      </c>
-      <c r="I28" s="4">
+      <c r="G28" s="4">
         <f t="shared" si="0"/>
         <v>0.13605878111760705</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D29" s="3">
         <v>4512</v>
@@ -1645,29 +1433,23 @@
       <c r="E29" s="5">
         <v>1.110343176632697</v>
       </c>
-      <c r="F29" s="13">
-        <v>1.090396959539798</v>
-      </c>
-      <c r="G29" s="5">
-        <v>1.110343176632697</v>
-      </c>
-      <c r="H29" s="13">
+      <c r="F29" s="12">
         <v>1.0903969595398</v>
       </c>
-      <c r="I29" s="4">
+      <c r="G29" s="4">
         <f t="shared" si="0"/>
         <v>-1.9946217092897012E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D30" s="7">
         <v>4512</v>
@@ -1675,29 +1457,23 @@
       <c r="E30" s="8">
         <v>1.6427863217142289</v>
       </c>
-      <c r="F30" s="15">
-        <v>6.1214364610666001</v>
-      </c>
-      <c r="G30" s="8">
-        <v>1.6427863217142289</v>
-      </c>
-      <c r="H30" s="22">
+      <c r="F30" s="14">
         <v>1.75</v>
       </c>
-      <c r="I30" s="4">
+      <c r="G30" s="4">
         <f t="shared" si="0"/>
         <v>0.10721367828577111</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D31" s="3">
         <v>8235</v>
@@ -1705,29 +1481,23 @@
       <c r="E31" s="5">
         <v>0.99984812652142507</v>
       </c>
-      <c r="F31" s="13">
-        <v>0.93856868295468066</v>
-      </c>
-      <c r="G31" s="5">
-        <v>0.99984812652142507</v>
-      </c>
-      <c r="H31" s="5">
+      <c r="F31" s="5">
         <v>0.93856868287683193</v>
       </c>
-      <c r="I31" s="4">
+      <c r="G31" s="4">
         <f t="shared" si="0"/>
         <v>-6.1279443644593146E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="D32" s="7">
         <v>8235</v>
@@ -1735,29 +1505,23 @@
       <c r="E32" s="8">
         <v>1.3509183278571011</v>
       </c>
-      <c r="F32" s="15">
-        <v>1.1038085988762949</v>
-      </c>
-      <c r="G32" s="8">
-        <v>1.1038085988762949</v>
-      </c>
-      <c r="H32" s="8">
+      <c r="F32" s="8">
         <v>1.1038086071662501</v>
       </c>
-      <c r="I32" s="4">
+      <c r="G32" s="4">
         <f t="shared" si="0"/>
         <v>-0.24710972069085102</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D33" s="3">
         <v>8235</v>
@@ -1765,29 +1529,23 @@
       <c r="E33" s="5">
         <v>0.71911700001927747</v>
       </c>
-      <c r="F33" s="13">
-        <v>0.69999925874019275</v>
-      </c>
-      <c r="G33" s="5">
-        <v>0.71911700001927747</v>
-      </c>
-      <c r="H33" s="5">
+      <c r="F33" s="5">
         <v>0.69999925868429502</v>
       </c>
-      <c r="I33" s="4">
+      <c r="G33" s="4">
         <f t="shared" si="0"/>
         <v>-1.9117741334982452E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D34" s="7">
         <v>8235</v>
@@ -1795,29 +1553,23 @@
       <c r="E34" s="8">
         <v>0.99999300082511844</v>
       </c>
-      <c r="F34" s="15">
-        <v>1.138682291755128</v>
-      </c>
-      <c r="G34" s="8">
-        <v>1.13868229175513</v>
-      </c>
-      <c r="H34" s="8">
+      <c r="F34" s="8">
         <v>1.13868229168991</v>
       </c>
-      <c r="I34" s="4">
+      <c r="G34" s="4">
         <f t="shared" si="0"/>
         <v>0.13868929086479154</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D35" s="3">
         <v>1039</v>
@@ -1825,24 +1577,18 @@
       <c r="E35" s="5">
         <v>1</v>
       </c>
-      <c r="F35" s="13">
-        <v>1.2109948087935949</v>
-      </c>
-      <c r="G35" s="5">
-        <v>1.21099480879359</v>
-      </c>
-      <c r="H35" s="5">
+      <c r="F35" s="5">
         <v>1.1479462828518601</v>
       </c>
-      <c r="I35" s="4">
+      <c r="G35" s="4">
         <f t="shared" si="0"/>
         <v>0.14794628285186007</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I35" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:G35" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D35">
     <cfRule type="colorScale" priority="2">
@@ -1856,7 +1602,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I35">
+  <conditionalFormatting sqref="G3:G35">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="-0.5"/>
@@ -1875,11 +1621,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,26 +1634,22 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1924,24 +1666,18 @@
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3">
@@ -1950,26 +1686,20 @@
       <c r="E3" s="5">
         <v>0.86212574269417985</v>
       </c>
-      <c r="F3" s="19">
-        <v>1.2198392667436351</v>
-      </c>
-      <c r="G3" s="11">
+      <c r="F3" s="11">
         <v>1.105</v>
       </c>
-      <c r="H3" s="11">
-        <v>1.105</v>
-      </c>
-      <c r="I3" s="4">
-        <f>H3-E3</f>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G32" si="0">F3-E3</f>
         <v>0.24287425730582013</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3">
@@ -1978,29 +1708,23 @@
       <c r="E4" s="5">
         <v>0.86212922230984146</v>
       </c>
-      <c r="F4" s="19">
-        <v>1.2198392667436351</v>
-      </c>
-      <c r="G4" s="11">
+      <c r="F4" s="11">
         <v>1.75</v>
       </c>
-      <c r="H4" s="11">
-        <v>1.75</v>
-      </c>
-      <c r="I4" s="4">
-        <f t="shared" ref="I4:I32" si="0">H4-E4</f>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
         <v>0.88787077769015854</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" s="7">
         <v>250000</v>
@@ -2008,29 +1732,23 @@
       <c r="E5" s="8">
         <v>1.194505303873032</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="11">
         <v>1.361</v>
       </c>
-      <c r="G5" s="11">
-        <v>1.361</v>
-      </c>
-      <c r="H5" s="11">
-        <v>1.361</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="G5" s="4">
         <f t="shared" si="0"/>
         <v>0.16649469612696799</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" s="7">
         <v>250000</v>
@@ -2038,29 +1756,23 @@
       <c r="E6" s="8">
         <v>1.194505303873032</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="11">
         <v>0.96399999999999997</v>
       </c>
-      <c r="G6" s="11">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="H6" s="11">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="I6" s="4">
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>-0.23050530387303203</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D7" s="3">
         <v>62331</v>
@@ -2068,29 +1780,23 @@
       <c r="E7" s="5">
         <v>0.78791720762815609</v>
       </c>
-      <c r="F7" s="19">
-        <v>0.77002156693463986</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.78791720762815609</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.78791720762815609</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="5">
+        <v>0.77</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.7917207628156073E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="D8" s="7">
         <v>62331</v>
@@ -2098,29 +1804,23 @@
       <c r="E8" s="8">
         <v>1.4532100920483779</v>
       </c>
-      <c r="F8" s="20">
-        <v>1.4234746248554611</v>
-      </c>
-      <c r="G8" s="8">
-        <v>1.4532100920483779</v>
-      </c>
-      <c r="H8" s="8">
-        <v>1.4532100920483779</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F8" s="8">
+        <v>1.423</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.0210092048377879E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3">
         <v>62331</v>
@@ -2128,29 +1828,23 @@
       <c r="E9" s="5">
         <v>0.58943073964021842</v>
       </c>
-      <c r="F9" s="19">
-        <v>0.66128277865653784</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0.58943073964021842</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.58943073964021842</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F9" s="5">
+        <v>0.65630256646670104</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>6.6871826826482628E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" s="7">
         <v>15823</v>
@@ -2158,29 +1852,23 @@
       <c r="E10" s="8">
         <v>0.97978032386560943</v>
       </c>
-      <c r="F10" s="20">
-        <v>0.88759591484851674</v>
-      </c>
-      <c r="G10" s="8">
+      <c r="F10" s="8">
         <v>0.88759591484851696</v>
       </c>
-      <c r="H10" s="8">
-        <v>0.88759591484851696</v>
-      </c>
-      <c r="I10" s="4">
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>-9.2184409017092461E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D11" s="3">
         <v>15823</v>
@@ -2191,26 +1879,20 @@
       <c r="F11" s="5">
         <v>1.0000973953997321</v>
       </c>
-      <c r="G11" s="5">
-        <v>1.0000973953997321</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1.0000973953997321</v>
-      </c>
-      <c r="I11" s="4">
+      <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>-2.1050296550972902E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" s="7">
         <v>15823</v>
@@ -2219,28 +1901,22 @@
         <v>0.99986363775758824</v>
       </c>
       <c r="F12" s="8">
-        <v>1.0141474866221261</v>
-      </c>
-      <c r="G12" s="8">
-        <v>0.99986363775758824</v>
-      </c>
-      <c r="H12" s="8">
-        <v>0.99986363775758824</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.014</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4136362242411771E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" s="3">
         <v>15823</v>
@@ -2249,28 +1925,22 @@
         <v>1.1101939672870871</v>
       </c>
       <c r="F13" s="5">
-        <v>1.1668831147892831</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1.1101939672870871</v>
-      </c>
-      <c r="H13" s="5">
-        <v>1.1101939672870871</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.167</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>5.6806032712912957E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14" s="7">
         <v>15823</v>
@@ -2279,28 +1949,22 @@
         <v>0.62047584909526032</v>
       </c>
       <c r="F14" s="8">
-        <v>0.39252693080556322</v>
-      </c>
-      <c r="G14" s="8">
         <v>0.392526930805563</v>
       </c>
-      <c r="H14" s="8">
-        <v>0.392526930805563</v>
-      </c>
-      <c r="I14" s="4">
+      <c r="G14" s="4">
         <f t="shared" si="0"/>
         <v>-0.22794891828969732</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D15" s="3">
         <v>19012</v>
@@ -2309,28 +1973,22 @@
         <v>0.9797969141258418</v>
       </c>
       <c r="F15" s="5">
-        <v>0.89398782046780623</v>
-      </c>
-      <c r="G15" s="5">
         <v>0.893987820467806</v>
       </c>
-      <c r="H15" s="5">
-        <v>0.893987820467806</v>
-      </c>
-      <c r="I15" s="4">
+      <c r="G15" s="4">
         <f t="shared" si="0"/>
         <v>-8.5809093658035795E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="D16" s="7">
         <v>19012</v>
@@ -2339,28 +1997,22 @@
         <v>1.031356637387876</v>
       </c>
       <c r="F16" s="8">
-        <v>1.0109425593271359</v>
-      </c>
-      <c r="G16" s="8">
-        <v>1.031356637387876</v>
-      </c>
-      <c r="H16" s="8">
-        <v>1.031356637387876</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>-2.0356637387876075E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D17" s="3">
         <v>19012</v>
@@ -2369,28 +2021,22 @@
         <v>0.93554043924404817</v>
       </c>
       <c r="F17" s="5">
-        <v>0.91873564059492485</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0.93554043924404817</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0.93554043924404817</v>
-      </c>
-      <c r="I17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.6540439244048133E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D18" s="7">
         <v>19012</v>
@@ -2399,28 +2045,22 @@
         <v>0.91087437801685334</v>
       </c>
       <c r="F18" s="8">
-        <v>0.78832227569992097</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0.78832227569992097</v>
-      </c>
-      <c r="H18" s="8">
-        <v>0.78832227569992097</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" si="0"/>
-        <v>-0.12255210231693237</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.86543611129386899</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="0"/>
+        <v>-4.5438266722984344E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" s="3">
         <v>19012</v>
@@ -2429,28 +2069,22 @@
         <v>1.0199397031365021</v>
       </c>
       <c r="F19" s="5">
-        <v>1.0561866341376711</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1.05618663413767</v>
-      </c>
-      <c r="H19" s="5">
-        <v>1.05618663413767</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="0"/>
-        <v>3.6246931001167937E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.056</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="0"/>
+        <v>3.6060296863497987E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D20" s="7">
         <v>19012</v>
@@ -2459,28 +2093,22 @@
         <v>1.0199526079424901</v>
       </c>
       <c r="F20" s="8">
-        <v>1.0407905370026611</v>
-      </c>
-      <c r="G20" s="8">
-        <v>1.0407905370026611</v>
-      </c>
-      <c r="H20" s="8">
-        <v>1.0407905370026611</v>
-      </c>
-      <c r="I20" s="4">
-        <f t="shared" si="0"/>
-        <v>2.0837929060171012E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.056</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="0"/>
+        <v>3.6047392057509953E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D21" s="3">
         <v>19012</v>
@@ -2489,28 +2117,22 @@
         <v>1.1745636239788431</v>
       </c>
       <c r="F21" s="5">
-        <v>1.1684944734748239</v>
-      </c>
-      <c r="G21" s="5">
-        <v>1.1745636239788431</v>
-      </c>
-      <c r="H21" s="5">
-        <v>1.1745636239788431</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="0"/>
+        <v>-6.5636239788431361E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D22" s="7">
         <v>19012</v>
@@ -2518,29 +2140,23 @@
       <c r="E22" s="8">
         <v>1.6240864380587079</v>
       </c>
-      <c r="F22" s="8">
-        <v>4.1537762141474852</v>
-      </c>
-      <c r="G22" s="8">
-        <v>1.6240864380587079</v>
-      </c>
-      <c r="H22" s="22">
+      <c r="F22" s="14">
         <v>1.75</v>
       </c>
-      <c r="I22" s="4">
+      <c r="G22" s="4">
         <f t="shared" si="0"/>
         <v>0.12591356194129211</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D23" s="3">
         <v>5118</v>
@@ -2549,28 +2165,22 @@
         <v>0.81268943647315883</v>
       </c>
       <c r="F23" s="5">
-        <v>0.7914753128417763</v>
-      </c>
-      <c r="G23" s="5">
-        <v>0.81268943647315883</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0.79147531284176431</v>
-      </c>
-      <c r="I23" s="4">
-        <f t="shared" si="0"/>
-        <v>-2.1214123631394521E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="0"/>
+        <v>-2.1689436473158796E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="D24" s="7">
         <v>5118</v>
@@ -2579,28 +2189,22 @@
         <v>0.58048435694307299</v>
       </c>
       <c r="F24" s="8">
-        <v>0.54903278599787875</v>
-      </c>
-      <c r="G24" s="8">
-        <v>0.58048435694307299</v>
-      </c>
-      <c r="H24" s="8">
-        <v>0.54903278599787719</v>
-      </c>
-      <c r="I24" s="4">
-        <f t="shared" si="0"/>
-        <v>-3.1451570945195795E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.1484356943072944E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D25" s="3">
         <v>5118</v>
@@ -2609,28 +2213,22 @@
         <v>0.60431452922472229</v>
       </c>
       <c r="F25" s="5">
-        <v>0.5226772929334651</v>
-      </c>
-      <c r="G25" s="5">
-        <v>0.52267729293346499</v>
-      </c>
-      <c r="H25" s="5">
-        <v>0.52267729293346599</v>
-      </c>
-      <c r="I25" s="4">
-        <f t="shared" si="0"/>
-        <v>-8.1637236291256299E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.52800129474999102</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.6313234474731262E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D26" s="7">
         <v>5118</v>
@@ -2639,28 +2237,22 @@
         <v>1.0001396385907659</v>
       </c>
       <c r="F26" s="8">
-        <v>1.0624107743185329</v>
-      </c>
-      <c r="G26" s="8">
-        <v>1</v>
-      </c>
-      <c r="H26" s="8">
-        <v>1.0624107743185323</v>
-      </c>
-      <c r="I26" s="4">
-        <f t="shared" si="0"/>
-        <v>6.2271135727766325E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.92018693217569703</v>
+      </c>
+      <c r="G26" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.9952706415068908E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D27" s="3">
         <v>5118</v>
@@ -2669,28 +2261,22 @@
         <v>1.466468130908914</v>
       </c>
       <c r="F27" s="5">
-        <v>1.320004151436504</v>
-      </c>
-      <c r="G27" s="5">
         <v>1.3200041514365</v>
       </c>
-      <c r="H27" s="5">
-        <v>1.3200041514365</v>
-      </c>
-      <c r="I27" s="4">
+      <c r="G27" s="4">
         <f t="shared" si="0"/>
         <v>-0.14646397947241407</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" s="7">
         <v>5118</v>
@@ -2698,29 +2284,23 @@
       <c r="E28" s="8">
         <v>1.6370254731010681</v>
       </c>
-      <c r="F28" s="8">
-        <v>4.6777567883175477</v>
-      </c>
-      <c r="G28" s="8">
-        <v>1.6370254731010681</v>
-      </c>
-      <c r="H28" s="22">
+      <c r="F28" s="14">
         <v>1.75</v>
       </c>
-      <c r="I28" s="4">
+      <c r="G28" s="4">
         <f t="shared" si="0"/>
         <v>0.11297452689893195</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D29" s="3">
         <v>3716</v>
@@ -2729,28 +2309,22 @@
         <v>1.00001060047308</v>
       </c>
       <c r="F29" s="5">
-        <v>1.493000983147607</v>
-      </c>
-      <c r="G29" s="5">
-        <v>1.00001060047308</v>
-      </c>
-      <c r="H29" s="5">
         <v>0.93856868287683193</v>
       </c>
-      <c r="I29" s="4">
+      <c r="G29" s="4">
         <f t="shared" si="0"/>
         <v>-6.1441917596248063E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D30" s="7">
         <v>3716</v>
@@ -2758,29 +2332,23 @@
       <c r="E30" s="8">
         <v>0.71883450621597023</v>
       </c>
-      <c r="F30" s="8">
-        <v>0.81648190410920141</v>
-      </c>
-      <c r="G30" s="8">
-        <v>0.71883450621597023</v>
-      </c>
-      <c r="H30" s="5">
+      <c r="F30" s="5">
         <v>0.6999992586842948</v>
       </c>
-      <c r="I30" s="4">
+      <c r="G30" s="4">
         <f t="shared" si="0"/>
         <v>-1.8835247531675425E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D31" s="3">
         <v>3716</v>
@@ -2788,29 +2356,23 @@
       <c r="E31" s="5">
         <v>1.000030224257074</v>
       </c>
-      <c r="F31" s="5">
-        <v>0.53758784951450911</v>
-      </c>
-      <c r="G31" s="5">
-        <v>1.000030224257074</v>
-      </c>
-      <c r="H31" s="8">
+      <c r="F31" s="8">
         <v>1.1386822916899089</v>
       </c>
-      <c r="I31" s="4">
+      <c r="G31" s="4">
         <f t="shared" si="0"/>
         <v>0.13865206743283487</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D32" s="7">
         <v>762</v>
@@ -2819,23 +2381,17 @@
         <v>1</v>
       </c>
       <c r="F32" s="8">
-        <v>0.72995442818162026</v>
-      </c>
-      <c r="G32" s="8">
-        <v>0.72995442818162026</v>
-      </c>
-      <c r="H32" s="8">
-        <v>0.77181399091233505</v>
-      </c>
-      <c r="I32" s="4">
-        <f t="shared" si="0"/>
-        <v>-0.22818600908766495</v>
+        <v>0.76726095288401097</v>
+      </c>
+      <c r="G32" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.23273904711598903</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I32" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A2:G32" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D4">
     <cfRule type="colorScale" priority="5">
@@ -2873,7 +2429,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I32">
+  <conditionalFormatting sqref="G3:G32">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="-0.5"/>
@@ -2891,11 +2447,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2904,26 +2460,22 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2940,27 +2492,21 @@
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" s="10">
         <v>23682</v>
@@ -2968,29 +2514,23 @@
       <c r="E3" s="5">
         <v>1.46</v>
       </c>
-      <c r="F3" s="5">
-        <v>1.8757824494845647</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="F3" s="14">
         <v>1.75</v>
       </c>
-      <c r="H3" s="5">
-        <v>1.75</v>
-      </c>
-      <c r="I3" s="4">
-        <f>H3-E3</f>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G42" si="0">F3-E3</f>
         <v>0.29000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="10">
         <v>3625</v>
@@ -2998,29 +2538,23 @@
       <c r="E4" s="5">
         <v>1.35</v>
       </c>
-      <c r="F4" s="5">
-        <v>1.9090690073763774</v>
-      </c>
-      <c r="G4" s="5">
+      <c r="F4" s="14">
         <v>1.75</v>
       </c>
-      <c r="H4" s="5">
-        <v>1.75</v>
-      </c>
-      <c r="I4" s="4">
-        <f t="shared" ref="I4:I42" si="0">H4-E4</f>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
         <v>0.39999999999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="9">
         <v>10415</v>
@@ -3031,26 +2565,20 @@
       <c r="F5" s="8">
         <v>1.5429749863728117</v>
       </c>
-      <c r="G5" s="8">
-        <v>1.5429749863728117</v>
-      </c>
-      <c r="H5" s="8">
-        <v>1.5429749863728117</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="G5" s="4">
         <f t="shared" si="0"/>
         <v>0.37297498637281179</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="10">
         <v>1865</v>
@@ -3058,29 +2586,23 @@
       <c r="E6" s="5">
         <v>1.77</v>
       </c>
-      <c r="F6" s="5">
-        <v>2.9798324151035613</v>
-      </c>
-      <c r="G6" s="5">
+      <c r="F6" s="14">
         <v>1.75</v>
       </c>
-      <c r="H6" s="5">
-        <v>1.75</v>
-      </c>
-      <c r="I6" s="4">
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>-2.0000000000000018E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" s="9">
         <v>50062</v>
@@ -3091,26 +2613,20 @@
       <c r="F7" s="8">
         <v>1.1723423661324466</v>
       </c>
-      <c r="G7" s="8">
-        <v>1.1723423661324466</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1.1723423661324466</v>
-      </c>
-      <c r="I7" s="4">
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>0.12234236613244653</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D8" s="10">
         <v>11566</v>
@@ -3118,29 +2634,23 @@
       <c r="E8" s="5">
         <v>1.34</v>
       </c>
-      <c r="F8" s="5">
-        <v>2.3062879776210434</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1.75</v>
-      </c>
-      <c r="H8" s="5">
+      <c r="F8" s="14">
         <v>2</v>
       </c>
-      <c r="I8" s="4">
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>0.65999999999999992</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9" s="9">
         <v>16188</v>
@@ -3151,26 +2661,20 @@
       <c r="F9" s="8">
         <v>1.0203679822336391</v>
       </c>
-      <c r="G9" s="8">
-        <v>1.0203679822336391</v>
-      </c>
-      <c r="H9" s="8">
-        <v>1.0203679822336391</v>
-      </c>
-      <c r="I9" s="4">
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>5.0367982233639141E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" s="10">
         <v>20442</v>
@@ -3181,26 +2685,20 @@
       <c r="F10" s="5">
         <v>1.5286165142488224</v>
       </c>
-      <c r="G10" s="5">
-        <v>1.5286165142488224</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1.5286165142488224</v>
-      </c>
-      <c r="I10" s="4">
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>0.37861651424882248</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" s="9">
         <v>5255</v>
@@ -3211,26 +2709,20 @@
       <c r="F11" s="8">
         <v>1.235494837675347</v>
       </c>
-      <c r="G11" s="8">
-        <v>1.235494837675347</v>
-      </c>
-      <c r="H11" s="8">
-        <v>1.235494837675347</v>
-      </c>
-      <c r="I11" s="4">
+      <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>0.33549483767534694</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12" s="10">
         <v>23682</v>
@@ -3241,26 +2733,20 @@
       <c r="F12" s="5">
         <v>1.1669628555435489</v>
       </c>
-      <c r="G12" s="5">
-        <v>1.1669628555435489</v>
-      </c>
-      <c r="H12" s="5">
-        <v>1.1669628555435489</v>
-      </c>
-      <c r="I12" s="4">
+      <c r="G12" s="4">
         <f t="shared" si="0"/>
         <v>1.6962855543549038E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13" s="9">
         <v>3625</v>
@@ -3271,26 +2757,20 @@
       <c r="F13" s="8">
         <v>1.2422164313353015</v>
       </c>
-      <c r="G13" s="8">
-        <v>1.2422164313353015</v>
-      </c>
-      <c r="H13" s="8">
-        <v>1.2422164313353015</v>
-      </c>
-      <c r="I13" s="4">
+      <c r="G13" s="4">
         <f t="shared" si="0"/>
         <v>-7.7783568664698599E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D14" s="10">
         <v>10415</v>
@@ -3301,26 +2781,20 @@
       <c r="F14" s="5">
         <v>1.0878734295345482</v>
       </c>
-      <c r="G14" s="5">
-        <v>1.0878734295345482</v>
-      </c>
-      <c r="H14" s="5">
-        <v>1.0878734295345482</v>
-      </c>
-      <c r="I14" s="4">
+      <c r="G14" s="4">
         <f t="shared" si="0"/>
         <v>-0.15212657046545175</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15" s="9">
         <v>1865</v>
@@ -3331,26 +2805,20 @@
       <c r="F15" s="8">
         <v>1.0843300140348211</v>
       </c>
-      <c r="G15" s="8">
-        <v>1.0843300140348211</v>
-      </c>
-      <c r="H15" s="8">
-        <v>1.0843300140348211</v>
-      </c>
-      <c r="I15" s="4">
+      <c r="G15" s="4">
         <f t="shared" si="0"/>
         <v>-8.566998596517883E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D16" s="10">
         <v>50062</v>
@@ -3361,26 +2829,20 @@
       <c r="F16" s="5">
         <v>1.2095924767566302</v>
       </c>
-      <c r="G16" s="5">
-        <v>1.2095924767566302</v>
-      </c>
-      <c r="H16" s="5">
-        <v>1.2095924767566302</v>
-      </c>
-      <c r="I16" s="4">
+      <c r="G16" s="4">
         <f t="shared" si="0"/>
         <v>-3.0407523243369816E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D17" s="9">
         <v>11566</v>
@@ -3391,26 +2853,20 @@
       <c r="F17" s="8">
         <v>0.93914652849348201</v>
       </c>
-      <c r="G17" s="8">
-        <v>0.93914652849348201</v>
-      </c>
-      <c r="H17" s="8">
-        <v>0.93914652849348201</v>
-      </c>
-      <c r="I17" s="4">
+      <c r="G17" s="4">
         <f t="shared" si="0"/>
         <v>9.1465284934819646E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D18" s="10">
         <v>16188</v>
@@ -3421,26 +2877,20 @@
       <c r="F18" s="5">
         <v>1.350929273771875</v>
       </c>
-      <c r="G18" s="5">
-        <v>1.350929273771875</v>
-      </c>
-      <c r="H18" s="5">
-        <v>1.350929273771875</v>
-      </c>
-      <c r="I18" s="4">
+      <c r="G18" s="4">
         <f t="shared" si="0"/>
         <v>-4.9070726228124917E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D19" s="9">
         <v>20442</v>
@@ -3451,26 +2901,20 @@
       <c r="F19" s="8">
         <v>1.4233355426573264</v>
       </c>
-      <c r="G19" s="8">
-        <v>1.4233355426573264</v>
-      </c>
-      <c r="H19" s="8">
-        <v>1.4233355426573264</v>
-      </c>
-      <c r="I19" s="4">
+      <c r="G19" s="4">
         <f t="shared" si="0"/>
         <v>-9.6664457342673593E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D20" s="10">
         <v>5255</v>
@@ -3481,26 +2925,20 @@
       <c r="F20" s="5">
         <v>1.1061996645820804</v>
       </c>
-      <c r="G20" s="5">
-        <v>1.1061996645820804</v>
-      </c>
-      <c r="H20" s="5">
-        <v>1.1061996645820804</v>
-      </c>
-      <c r="I20" s="4">
+      <c r="G20" s="4">
         <f t="shared" si="0"/>
         <v>-8.3800335417919536E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D21" s="9">
         <v>3335</v>
@@ -3509,28 +2947,22 @@
         <v>0.85000307561054256</v>
       </c>
       <c r="F21" s="8">
-        <v>0.87032221285327571</v>
-      </c>
-      <c r="G21" s="8">
-        <v>0.85000307561054256</v>
-      </c>
-      <c r="H21" s="8">
-        <v>0.85000307561054256</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.87032221300000001</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="0"/>
+        <v>2.0319137389457453E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D22" s="10">
         <v>3335</v>
@@ -3539,28 +2971,22 @@
         <v>1.140000396796113</v>
       </c>
       <c r="F22" s="5">
-        <v>0.99725214336501611</v>
-      </c>
-      <c r="G22" s="5">
         <v>1</v>
       </c>
-      <c r="H22" s="5">
-        <v>1</v>
-      </c>
-      <c r="I22" s="4">
+      <c r="G22" s="4">
         <f t="shared" si="0"/>
         <v>-0.14000039679611298</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D23" s="9">
         <v>3335</v>
@@ -3569,28 +2995,22 @@
         <v>1.0000030845747501</v>
       </c>
       <c r="F23" s="8">
-        <v>1.136873199569439</v>
-      </c>
-      <c r="G23" s="8">
-        <v>1</v>
-      </c>
-      <c r="H23" s="8">
-        <v>1</v>
-      </c>
-      <c r="I23" s="4">
-        <f t="shared" si="0"/>
-        <v>-3.0845747500674037E-6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.13636363636363</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="0"/>
+        <v>0.13636055178887996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D24" s="10">
         <v>1254</v>
@@ -3599,28 +3019,22 @@
         <v>0.99999960448344705</v>
       </c>
       <c r="F24" s="5">
-        <v>0.93014062855326196</v>
-      </c>
-      <c r="G24" s="5">
-        <v>1</v>
-      </c>
-      <c r="H24" s="5">
-        <v>1</v>
-      </c>
-      <c r="I24" s="4">
-        <f t="shared" si="0"/>
-        <v>3.9551655295344545E-7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.93014062799999997</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" si="0"/>
+        <v>-6.9858976483447077E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="D25" s="9">
         <v>1254</v>
@@ -3631,26 +3045,20 @@
       <c r="F25" s="8">
         <v>1.0006734828099859</v>
       </c>
-      <c r="G25" s="8">
-        <v>1.0006734828099859</v>
-      </c>
-      <c r="H25" s="8">
-        <v>1.0006734828099859</v>
-      </c>
-      <c r="I25" s="4">
+      <c r="G25" s="4">
         <f t="shared" si="0"/>
         <v>0.16067285438703183</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D26" s="10">
         <v>1254</v>
@@ -3661,26 +3069,20 @@
       <c r="F26" s="5">
         <v>0.85450305494614942</v>
       </c>
-      <c r="G26" s="5">
-        <v>0.85450305494614942</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0.85450305494614942</v>
-      </c>
-      <c r="I26" s="4">
+      <c r="G26" s="4">
         <f t="shared" si="0"/>
         <v>-0.14549659318197672</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D27" s="9">
         <v>1254</v>
@@ -3691,26 +3093,20 @@
       <c r="F27" s="8">
         <v>1.2987776962568871</v>
       </c>
-      <c r="G27" s="8">
-        <v>1.2987776962568871</v>
-      </c>
-      <c r="H27" s="8">
-        <v>1.2987776962568871</v>
-      </c>
-      <c r="I27" s="4">
+      <c r="G27" s="4">
         <f t="shared" si="0"/>
         <v>0.29877802352304106</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D28" s="10">
         <v>1254</v>
@@ -3721,26 +3117,20 @@
       <c r="F28" s="5">
         <v>1</v>
       </c>
-      <c r="G28" s="5">
-        <v>1</v>
-      </c>
-      <c r="H28" s="5">
-        <v>1</v>
-      </c>
-      <c r="I28" s="4">
+      <c r="G28" s="4">
         <f t="shared" si="0"/>
         <v>1.0327147272892745E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D29" s="9">
         <v>1029</v>
@@ -3749,28 +3139,22 @@
         <v>1.0087302754317311</v>
       </c>
       <c r="F29" s="8">
-        <v>1.1119043724798301</v>
-      </c>
-      <c r="G29" s="8">
-        <v>1.0087302754317311</v>
-      </c>
-      <c r="H29" s="8">
         <v>1.09064438292682</v>
       </c>
-      <c r="I29" s="4">
+      <c r="G29" s="4">
         <f t="shared" si="0"/>
         <v>8.1914107495088873E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="D30" s="10">
         <v>1029</v>
@@ -3779,28 +3163,22 @@
         <v>1.5947861280203559</v>
       </c>
       <c r="F30" s="5">
-        <v>1.0917465999300731</v>
-      </c>
-      <c r="G30" s="5">
-        <v>1</v>
-      </c>
-      <c r="H30" s="5">
         <v>1.1651372000584399</v>
       </c>
-      <c r="I30" s="4">
+      <c r="G30" s="4">
         <f t="shared" si="0"/>
         <v>-0.42964892796191601</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D31" s="9">
         <v>1029</v>
@@ -3809,28 +3187,22 @@
         <v>1.3152958851067931</v>
       </c>
       <c r="F31" s="8">
-        <v>1.3349901497607559</v>
-      </c>
-      <c r="G31" s="8">
-        <v>1.3152958851067931</v>
-      </c>
-      <c r="H31" s="8">
         <v>1.3456222354051699</v>
       </c>
-      <c r="I31" s="4">
+      <c r="G31" s="4">
         <f t="shared" si="0"/>
         <v>3.0326350298376825E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D32" s="10">
         <v>1029</v>
@@ -3838,29 +3210,23 @@
       <c r="E32" s="5">
         <v>1.540662781470777</v>
       </c>
-      <c r="F32" s="5">
-        <v>1.4794191914320529</v>
-      </c>
-      <c r="G32" s="5">
-        <v>1.540662781470777</v>
-      </c>
-      <c r="H32" s="5">
-        <v>1.60625232365774</v>
-      </c>
-      <c r="I32" s="4">
-        <f t="shared" si="0"/>
-        <v>6.5589542186963001E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F32" s="8">
+        <v>1.86898239128154</v>
+      </c>
+      <c r="G32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.32831960981076302</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D33" s="9">
         <v>1029</v>
@@ -3869,28 +3235,22 @@
         <v>0.74075833503750932</v>
       </c>
       <c r="F33" s="8">
-        <v>0.73183402027207978</v>
-      </c>
-      <c r="G33" s="8">
-        <v>0.74075833503750932</v>
-      </c>
-      <c r="H33" s="8">
         <v>0.73706281062687995</v>
       </c>
-      <c r="I33" s="4">
+      <c r="G33" s="4">
         <f t="shared" si="0"/>
         <v>-3.6955244106293694E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D34" s="10">
         <v>1029</v>
@@ -3898,29 +3258,23 @@
       <c r="E34" s="5">
         <v>1.013286273165287</v>
       </c>
-      <c r="F34" s="5">
-        <v>0.85584306563848311</v>
-      </c>
-      <c r="G34" s="5">
-        <v>1.013286273165287</v>
-      </c>
-      <c r="H34" s="5">
-        <v>0.8548156544106621</v>
-      </c>
-      <c r="I34" s="4">
-        <f t="shared" si="0"/>
-        <v>-0.15847061875462487</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F34" s="8">
+        <v>0.73706281062687995</v>
+      </c>
+      <c r="G34" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.27622346253840702</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D35" s="9">
         <v>1029</v>
@@ -3929,28 +3283,22 @@
         <v>1.001803448301279</v>
       </c>
       <c r="F35" s="8">
-        <v>1.3329905566535889</v>
-      </c>
-      <c r="G35" s="8">
-        <v>1.001803448301279</v>
-      </c>
-      <c r="H35" s="8">
         <v>1.3359753183308014</v>
       </c>
-      <c r="I35" s="4">
+      <c r="G35" s="4">
         <f t="shared" si="0"/>
         <v>0.33417187002952242</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D36" s="10">
         <v>1029</v>
@@ -3958,29 +3306,23 @@
       <c r="E36" s="5">
         <v>0.35590806731908381</v>
       </c>
-      <c r="F36" s="5">
-        <v>8.0030786327040335E-3</v>
-      </c>
-      <c r="G36" s="5">
-        <v>0.35590806731908381</v>
-      </c>
-      <c r="H36" s="22">
+      <c r="F36" s="14">
         <v>0.25</v>
       </c>
-      <c r="I36" s="4">
+      <c r="G36" s="4">
         <f t="shared" si="0"/>
         <v>-0.10590806731908381</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D37" s="9">
         <v>287</v>
@@ -3989,28 +3331,22 @@
         <v>0.44462048265946652</v>
       </c>
       <c r="F37" s="8">
-        <v>0.23934946642919319</v>
-      </c>
-      <c r="G37" s="8">
-        <v>0.44462048265946652</v>
-      </c>
-      <c r="H37" s="8">
         <v>0.25</v>
       </c>
-      <c r="I37" s="4">
+      <c r="G37" s="4">
         <f t="shared" si="0"/>
         <v>-0.19462048265946652</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D38" s="10">
         <v>287</v>
@@ -4019,28 +3355,22 @@
         <v>0.98777793290015015</v>
       </c>
       <c r="F38" s="5">
-        <v>0.46248103037875571</v>
-      </c>
-      <c r="G38" s="5">
-        <v>0.98777793290015015</v>
-      </c>
-      <c r="H38" s="5">
-        <v>0.48833040506159497</v>
-      </c>
-      <c r="I38" s="4">
-        <f t="shared" si="0"/>
-        <v>-0.49944752783855517</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.49449930669672199</v>
+      </c>
+      <c r="G38" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.49327862620342816</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D39" s="9">
         <v>287</v>
@@ -4048,29 +3378,23 @@
       <c r="E39" s="8">
         <v>0.28616644412307951</v>
       </c>
-      <c r="F39" s="8">
-        <v>0.1108189009804959</v>
-      </c>
-      <c r="G39" s="8">
-        <v>0.28616644412307951</v>
-      </c>
-      <c r="H39" s="8">
-        <v>0.12352640223107059</v>
-      </c>
-      <c r="I39" s="4">
-        <f t="shared" si="0"/>
-        <v>-0.16264004189200892</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F39" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G39" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.6166444123079511E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D40" s="10">
         <v>287</v>
@@ -4079,28 +3403,22 @@
         <v>1.084432142232894</v>
       </c>
       <c r="F40" s="5">
-        <v>0.9207851015115387</v>
-      </c>
-      <c r="G40" s="5">
-        <v>1</v>
-      </c>
-      <c r="H40" s="5">
-        <v>0.93758507353810205</v>
-      </c>
-      <c r="I40" s="4">
-        <f t="shared" si="0"/>
-        <v>-0.14684706869479192</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="G40" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.41743214223289393</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D41" s="9">
         <v>287</v>
@@ -4109,28 +3427,22 @@
         <v>1.0009148071180201</v>
       </c>
       <c r="F41" s="8">
-        <v>0.83422811425921606</v>
-      </c>
-      <c r="G41" s="8">
-        <v>1</v>
-      </c>
-      <c r="H41" s="8">
         <v>1.0957770660791699</v>
       </c>
-      <c r="I41" s="4">
+      <c r="G41" s="4">
         <f t="shared" si="0"/>
         <v>9.4862258961149859E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D42" s="10">
         <v>287</v>
@@ -4138,26 +3450,20 @@
       <c r="E42" s="5">
         <v>0.35328227106859889</v>
       </c>
-      <c r="F42" s="5">
-        <v>6.6188493453385899E-2</v>
-      </c>
-      <c r="G42" s="5">
-        <v>0.35328227106859889</v>
-      </c>
-      <c r="H42" s="22">
+      <c r="F42" s="14">
         <v>0.25</v>
       </c>
-      <c r="I42" s="4">
+      <c r="G42" s="4">
         <f t="shared" si="0"/>
         <v>-0.10328227106859889</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I42" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A2:G42" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D3:D42">
     <cfRule type="colorScale" priority="15">
       <colorScale>
@@ -4170,7 +3476,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I42">
+  <conditionalFormatting sqref="G3:G42">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="-0.5"/>

</xml_diff>